<commit_message>
Control unit was only 12 valid states
</commit_message>
<xml_diff>
--- a/Microprocessor.xlsx
+++ b/Microprocessor.xlsx
@@ -271,7 +271,7 @@
     <t xml:space="preserve">disp15</t>
   </si>
   <si>
-    <t xml:space="preserve">FO-disp15</t>
+    <t xml:space="preserve">CI-disp15</t>
   </si>
   <si>
     <t xml:space="preserve">IP-next</t>
@@ -332,7 +332,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -391,6 +391,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDAE3F3"/>
         <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -687,7 +693,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="163">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1208,75 +1214,135 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="33" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="20" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="34" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="35" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="36" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="22" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="33" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="20" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="34" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="35" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="36" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="11" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="22" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="11" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="17" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1360,7 +1426,7 @@
   <dimension ref="1:27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y24" activeCellId="0" sqref="Y24"/>
+      <selection pane="topLeft" activeCell="AZ25" activeCellId="0" sqref="AZ25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -5088,7 +5154,7 @@
       <c r="AY24" s="134" t="n">
         <v>0</v>
       </c>
-      <c r="AZ24" s="104" t="n">
+      <c r="AZ24" s="140" t="n">
         <v>0</v>
       </c>
       <c r="BA24" s="137" t="n">
@@ -5108,491 +5174,491 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="108" t="s">
+      <c r="A25" s="141" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="140" t="s">
+      <c r="B25" s="142" t="s">
         <v>83</v>
       </c>
-      <c r="C25" s="141" t="s">
-        <v>37</v>
-      </c>
-      <c r="D25" s="140" t="s">
-        <v>37</v>
-      </c>
-      <c r="E25" s="140" t="s">
-        <v>37</v>
-      </c>
-      <c r="F25" s="140" t="s">
-        <v>37</v>
-      </c>
-      <c r="G25" s="142" t="s">
-        <v>37</v>
-      </c>
-      <c r="H25" s="143" t="n">
-        <v>1</v>
-      </c>
-      <c r="I25" s="141" t="s">
+      <c r="C25" s="143" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="142" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="142" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25" s="142" t="s">
+        <v>37</v>
+      </c>
+      <c r="G25" s="144" t="s">
+        <v>37</v>
+      </c>
+      <c r="H25" s="141" t="n">
+        <v>1</v>
+      </c>
+      <c r="I25" s="143" t="s">
         <v>82</v>
       </c>
-      <c r="J25" s="141"/>
-      <c r="K25" s="141"/>
-      <c r="L25" s="141"/>
-      <c r="M25" s="141"/>
-      <c r="N25" s="141"/>
-      <c r="O25" s="141"/>
-      <c r="P25" s="141"/>
-      <c r="Q25" s="141"/>
-      <c r="R25" s="141"/>
-      <c r="S25" s="141"/>
-      <c r="T25" s="141"/>
-      <c r="U25" s="141"/>
-      <c r="V25" s="141"/>
-      <c r="W25" s="141"/>
-      <c r="X25" s="122" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y25" s="140" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z25" s="140" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA25" s="140" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB25" s="140" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC25" s="140" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD25" s="140" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE25" s="140" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF25" s="140" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG25" s="140" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH25" s="140" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI25" s="140" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ25" s="142" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK25" s="141" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL25" s="140" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM25" s="140" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN25" s="142" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO25" s="141" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP25" s="140" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ25" s="140" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR25" s="142" t="n">
-        <v>1</v>
-      </c>
-      <c r="AS25" s="141" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT25" s="140" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU25" s="140" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV25" s="142" t="n">
-        <v>1</v>
-      </c>
-      <c r="AW25" s="143" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX25" s="140" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY25" s="143" t="n">
-        <v>0</v>
-      </c>
-      <c r="AZ25" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA25" s="141" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB25" s="140" t="n">
-        <v>1</v>
-      </c>
-      <c r="BC25" s="140" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD25" s="142" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE25" s="142" t="n">
+      <c r="J25" s="143"/>
+      <c r="K25" s="143"/>
+      <c r="L25" s="143"/>
+      <c r="M25" s="143"/>
+      <c r="N25" s="143"/>
+      <c r="O25" s="143"/>
+      <c r="P25" s="143"/>
+      <c r="Q25" s="143"/>
+      <c r="R25" s="143"/>
+      <c r="S25" s="143"/>
+      <c r="T25" s="143"/>
+      <c r="U25" s="143"/>
+      <c r="V25" s="143"/>
+      <c r="W25" s="143"/>
+      <c r="X25" s="145" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y25" s="142" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z25" s="142" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA25" s="142" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB25" s="142" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC25" s="142" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD25" s="142" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE25" s="142" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF25" s="142" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG25" s="142" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH25" s="142" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI25" s="142" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ25" s="144" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK25" s="143" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL25" s="142" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM25" s="142" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN25" s="144" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO25" s="143" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP25" s="142" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ25" s="142" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR25" s="144" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS25" s="143" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT25" s="142" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU25" s="142" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV25" s="144" t="n">
+        <v>1</v>
+      </c>
+      <c r="AW25" s="141" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX25" s="142" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY25" s="141" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ25" s="146" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA25" s="143" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB25" s="142" t="n">
+        <v>1</v>
+      </c>
+      <c r="BC25" s="142" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD25" s="144" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE25" s="144" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="108" t="s">
+      <c r="A26" s="141" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="101" t="s">
+      <c r="B26" s="147" t="s">
         <v>84</v>
       </c>
-      <c r="C26" s="144" t="n">
-        <v>0</v>
-      </c>
-      <c r="D26" s="96" t="s">
-        <v>37</v>
-      </c>
-      <c r="E26" s="96" t="s">
-        <v>37</v>
-      </c>
-      <c r="F26" s="96" t="s">
-        <v>37</v>
-      </c>
-      <c r="G26" s="96" t="s">
-        <v>37</v>
-      </c>
-      <c r="H26" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="I26" s="55" t="s">
-        <v>37</v>
-      </c>
-      <c r="J26" s="96" t="s">
-        <v>37</v>
-      </c>
-      <c r="K26" s="96" t="s">
-        <v>37</v>
-      </c>
-      <c r="L26" s="96" t="s">
-        <v>37</v>
-      </c>
-      <c r="M26" s="96" t="s">
-        <v>37</v>
-      </c>
-      <c r="N26" s="96" t="s">
-        <v>37</v>
-      </c>
-      <c r="O26" s="96" t="s">
-        <v>37</v>
-      </c>
-      <c r="P26" s="96" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q26" s="96" t="s">
-        <v>37</v>
-      </c>
-      <c r="R26" s="96" t="s">
-        <v>37</v>
-      </c>
-      <c r="S26" s="96" t="s">
-        <v>37</v>
-      </c>
-      <c r="T26" s="96" t="s">
-        <v>37</v>
-      </c>
-      <c r="U26" s="96" t="s">
-        <v>37</v>
-      </c>
-      <c r="V26" s="96" t="s">
-        <v>37</v>
-      </c>
-      <c r="W26" s="96" t="s">
-        <v>37</v>
-      </c>
-      <c r="X26" s="98" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y26" s="96" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z26" s="96" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA26" s="96" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB26" s="96" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC26" s="96" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD26" s="96" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE26" s="96" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF26" s="96" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG26" s="96" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH26" s="96" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI26" s="96" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ26" s="96" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK26" s="144" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL26" s="96" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM26" s="96" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN26" s="96" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO26" s="144" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP26" s="96" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ26" s="96" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR26" s="96" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS26" s="144" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT26" s="96" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU26" s="96" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV26" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW26" s="145" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX26" s="146" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY26" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AZ26" s="60" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA26" s="146" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB26" s="96" t="n">
-        <v>1</v>
-      </c>
-      <c r="BC26" s="96" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD26" s="96" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE26" s="147" t="n">
+      <c r="C26" s="148" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="149" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" s="149" t="s">
+        <v>37</v>
+      </c>
+      <c r="F26" s="149" t="s">
+        <v>37</v>
+      </c>
+      <c r="G26" s="149" t="s">
+        <v>37</v>
+      </c>
+      <c r="H26" s="150" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" s="150" t="s">
+        <v>37</v>
+      </c>
+      <c r="J26" s="149" t="s">
+        <v>37</v>
+      </c>
+      <c r="K26" s="149" t="s">
+        <v>37</v>
+      </c>
+      <c r="L26" s="149" t="s">
+        <v>37</v>
+      </c>
+      <c r="M26" s="149" t="s">
+        <v>37</v>
+      </c>
+      <c r="N26" s="149" t="s">
+        <v>37</v>
+      </c>
+      <c r="O26" s="149" t="s">
+        <v>37</v>
+      </c>
+      <c r="P26" s="149" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q26" s="149" t="s">
+        <v>37</v>
+      </c>
+      <c r="R26" s="149" t="s">
+        <v>37</v>
+      </c>
+      <c r="S26" s="149" t="s">
+        <v>37</v>
+      </c>
+      <c r="T26" s="149" t="s">
+        <v>37</v>
+      </c>
+      <c r="U26" s="149" t="s">
+        <v>37</v>
+      </c>
+      <c r="V26" s="149" t="s">
+        <v>37</v>
+      </c>
+      <c r="W26" s="149" t="s">
+        <v>37</v>
+      </c>
+      <c r="X26" s="151" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y26" s="149" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="149" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA26" s="149" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB26" s="149" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC26" s="149" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD26" s="149" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE26" s="149" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF26" s="149" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG26" s="149" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH26" s="149" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI26" s="149" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ26" s="149" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK26" s="148" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL26" s="149" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM26" s="149" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN26" s="149" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO26" s="148" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP26" s="149" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ26" s="149" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR26" s="149" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS26" s="148" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT26" s="149" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU26" s="149" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV26" s="152" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW26" s="153" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX26" s="154" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY26" s="150" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ26" s="155" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA26" s="154" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB26" s="149" t="n">
+        <v>1</v>
+      </c>
+      <c r="BC26" s="149" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD26" s="149" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE26" s="156" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="108"/>
-      <c r="B27" s="128" t="s">
+      <c r="A27" s="141"/>
+      <c r="B27" s="157" t="s">
         <v>85</v>
       </c>
-      <c r="C27" s="119" t="n">
-        <v>1</v>
-      </c>
-      <c r="D27" s="118" t="s">
-        <v>37</v>
-      </c>
-      <c r="E27" s="118" t="s">
-        <v>37</v>
-      </c>
-      <c r="F27" s="118" t="s">
-        <v>37</v>
-      </c>
-      <c r="G27" s="120" t="s">
-        <v>37</v>
-      </c>
-      <c r="H27" s="122" t="n">
-        <v>0</v>
-      </c>
-      <c r="I27" s="119" t="s">
-        <v>37</v>
-      </c>
-      <c r="J27" s="118" t="s">
-        <v>37</v>
-      </c>
-      <c r="K27" s="118" t="s">
-        <v>37</v>
-      </c>
-      <c r="L27" s="118" t="s">
-        <v>37</v>
-      </c>
-      <c r="M27" s="118" t="s">
-        <v>37</v>
-      </c>
-      <c r="N27" s="118" t="s">
-        <v>37</v>
-      </c>
-      <c r="O27" s="118" t="s">
-        <v>37</v>
-      </c>
-      <c r="P27" s="118" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q27" s="118" t="s">
-        <v>37</v>
-      </c>
-      <c r="R27" s="118" t="s">
-        <v>37</v>
-      </c>
-      <c r="S27" s="118" t="s">
-        <v>37</v>
-      </c>
-      <c r="T27" s="118" t="s">
-        <v>37</v>
-      </c>
-      <c r="U27" s="118" t="s">
-        <v>37</v>
-      </c>
-      <c r="V27" s="118" t="s">
-        <v>37</v>
-      </c>
-      <c r="W27" s="118" t="s">
-        <v>37</v>
-      </c>
-      <c r="X27" s="122" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y27" s="118" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z27" s="118" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA27" s="118" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB27" s="118" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC27" s="118" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD27" s="118" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE27" s="118" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF27" s="118" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG27" s="118" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH27" s="118" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI27" s="118" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ27" s="120" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK27" s="119" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL27" s="118" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM27" s="118" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN27" s="120" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO27" s="119" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP27" s="118" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ27" s="118" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR27" s="120" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS27" s="119" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT27" s="118" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU27" s="118" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV27" s="120" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW27" s="121" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX27" s="118" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY27" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="AZ27" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA27" s="119" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB27" s="118" t="n">
-        <v>1</v>
-      </c>
-      <c r="BC27" s="118" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD27" s="120" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE27" s="120" t="n">
+      <c r="C27" s="158" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" s="159" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" s="159" t="s">
+        <v>37</v>
+      </c>
+      <c r="F27" s="159" t="s">
+        <v>37</v>
+      </c>
+      <c r="G27" s="160" t="s">
+        <v>37</v>
+      </c>
+      <c r="H27" s="145" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" s="158" t="s">
+        <v>37</v>
+      </c>
+      <c r="J27" s="159" t="s">
+        <v>37</v>
+      </c>
+      <c r="K27" s="159" t="s">
+        <v>37</v>
+      </c>
+      <c r="L27" s="159" t="s">
+        <v>37</v>
+      </c>
+      <c r="M27" s="159" t="s">
+        <v>37</v>
+      </c>
+      <c r="N27" s="159" t="s">
+        <v>37</v>
+      </c>
+      <c r="O27" s="159" t="s">
+        <v>37</v>
+      </c>
+      <c r="P27" s="159" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q27" s="159" t="s">
+        <v>37</v>
+      </c>
+      <c r="R27" s="159" t="s">
+        <v>37</v>
+      </c>
+      <c r="S27" s="159" t="s">
+        <v>37</v>
+      </c>
+      <c r="T27" s="159" t="s">
+        <v>37</v>
+      </c>
+      <c r="U27" s="159" t="s">
+        <v>37</v>
+      </c>
+      <c r="V27" s="159" t="s">
+        <v>37</v>
+      </c>
+      <c r="W27" s="159" t="s">
+        <v>37</v>
+      </c>
+      <c r="X27" s="145" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y27" s="159" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z27" s="159" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA27" s="159" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="159" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC27" s="159" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD27" s="159" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE27" s="159" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF27" s="159" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG27" s="159" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH27" s="159" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI27" s="159" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ27" s="160" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK27" s="158" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL27" s="159" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM27" s="159" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN27" s="160" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO27" s="158" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP27" s="159" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ27" s="159" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR27" s="160" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS27" s="158" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT27" s="159" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU27" s="159" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV27" s="160" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW27" s="161" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX27" s="159" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY27" s="162" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ27" s="146" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA27" s="158" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB27" s="159" t="n">
+        <v>1</v>
+      </c>
+      <c r="BC27" s="159" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD27" s="160" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE27" s="160" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bug en ble was repared
</commit_message>
<xml_diff>
--- a/Microprocessor.xlsx
+++ b/Microprocessor.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="92">
   <si>
     <t xml:space="preserve">State</t>
   </si>
@@ -253,10 +253,13 @@
     <t xml:space="preserve">disp8</t>
   </si>
   <si>
-    <t xml:space="preserve">EW-jump</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EW-branch</t>
+    <t xml:space="preserve">sign ext</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EW-jb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mov</t>
   </si>
   <si>
     <t xml:space="preserve">FO-stlimm8</t>
@@ -308,6 +311,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -330,17 +334,20 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="11">
@@ -1180,28 +1187,12 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="9" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="10" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1236,6 +1227,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1316,11 +1311,23 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="38" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="9" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1441,10 +1448,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:29"/>
+  <dimension ref="1:27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AD1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22:I22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AY17" activeCellId="0" sqref="AY17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3816,7 +3823,7 @@
         <v>1</v>
       </c>
       <c r="AO16" s="71" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP16" s="72" t="n">
         <v>0</v>
@@ -3825,7 +3832,7 @@
         <v>0</v>
       </c>
       <c r="AR16" s="73" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS16" s="71" t="n">
         <v>1</v>
@@ -3852,19 +3859,22 @@
         <v>0</v>
       </c>
       <c r="BA16" s="71" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB16" s="72" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC16" s="72" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD16" s="73" t="n">
         <v>0</v>
       </c>
       <c r="BE16" s="73" t="n">
         <v>0</v>
+      </c>
+      <c r="BF16" s="0" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3872,7 +3882,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="86" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C17" s="45" t="s">
         <v>37</v>
@@ -3913,8 +3923,8 @@
       <c r="O17" s="66" t="n">
         <v>0</v>
       </c>
-      <c r="P17" s="70" t="n">
-        <v>0</v>
+      <c r="P17" s="70" t="s">
+        <v>37</v>
       </c>
       <c r="Q17" s="45" t="s">
         <v>37</v>
@@ -3977,16 +3987,16 @@
         <v>0</v>
       </c>
       <c r="AK17" s="46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL17" s="45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM17" s="45" t="n">
         <v>0</v>
       </c>
       <c r="AN17" s="47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO17" s="46" t="n">
         <v>1</v>
@@ -4018,11 +4028,11 @@
       <c r="AX17" s="45" t="n">
         <v>0</v>
       </c>
-      <c r="AY17" s="69" t="s">
-        <v>37</v>
-      </c>
-      <c r="AZ17" s="66" t="s">
-        <v>37</v>
+      <c r="AY17" s="68" t="s">
+        <v>37</v>
+      </c>
+      <c r="AZ17" s="115" t="n">
+        <v>1</v>
       </c>
       <c r="BA17" s="46" t="n">
         <v>0</v>
@@ -4034,352 +4044,329 @@
         <v>0</v>
       </c>
       <c r="BD17" s="47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE17" s="47" t="n">
         <v>0</v>
+      </c>
+      <c r="BF17" s="116" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="113"/>
-      <c r="B18" s="105" t="s">
-        <v>78</v>
-      </c>
-      <c r="C18" s="97" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="97" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="97" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="97" t="s">
-        <v>15</v>
-      </c>
-      <c r="G18" s="98" t="s">
-        <v>16</v>
-      </c>
-      <c r="H18" s="104" t="n">
-        <v>0</v>
-      </c>
-      <c r="I18" s="115" t="n">
-        <v>1</v>
-      </c>
-      <c r="J18" s="104" t="n">
-        <v>0</v>
-      </c>
-      <c r="K18" s="104" t="n">
-        <v>0</v>
-      </c>
-      <c r="L18" s="104" t="n">
-        <v>1</v>
-      </c>
-      <c r="M18" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="N18" s="115"/>
-      <c r="O18" s="115"/>
-      <c r="P18" s="116" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="97" t="s">
-        <v>37</v>
-      </c>
-      <c r="R18" s="97" t="s">
-        <v>37</v>
-      </c>
-      <c r="S18" s="97" t="s">
-        <v>37</v>
-      </c>
-      <c r="T18" s="97" t="s">
-        <v>37</v>
-      </c>
-      <c r="U18" s="97" t="s">
-        <v>37</v>
-      </c>
-      <c r="V18" s="97" t="s">
-        <v>37</v>
-      </c>
-      <c r="W18" s="117" t="n">
-        <v>0</v>
-      </c>
-      <c r="X18" s="116" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y18" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z18" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA18" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB18" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC18" s="97" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD18" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE18" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF18" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG18" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH18" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI18" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ18" s="98" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK18" s="118" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL18" s="97" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM18" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN18" s="98" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO18" s="118" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP18" s="97" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ18" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR18" s="98" t="n">
-        <v>1</v>
-      </c>
-      <c r="AS18" s="118" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT18" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU18" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV18" s="98" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW18" s="119" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX18" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY18" s="119" t="s">
-        <v>37</v>
-      </c>
-      <c r="AZ18" s="104" t="s">
-        <v>37</v>
-      </c>
-      <c r="BA18" s="118" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB18" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC18" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD18" s="98" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE18" s="98" t="n">
+      <c r="A18" s="78" t="n">
+        <v>8</v>
+      </c>
+      <c r="B18" s="61" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="55" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" s="57" t="s">
+        <v>37</v>
+      </c>
+      <c r="H18" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="J18" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="L18" s="57" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" s="61" t="s">
+        <v>43</v>
+      </c>
+      <c r="N18" s="61"/>
+      <c r="O18" s="61"/>
+      <c r="P18" s="55" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q18" s="55"/>
+      <c r="R18" s="55"/>
+      <c r="S18" s="55"/>
+      <c r="T18" s="55"/>
+      <c r="U18" s="55"/>
+      <c r="V18" s="55"/>
+      <c r="W18" s="55"/>
+      <c r="X18" s="117" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC18" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD18" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF18" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG18" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH18" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI18" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ18" s="57" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK18" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL18" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM18" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN18" s="57" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO18" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP18" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ18" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR18" s="57" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS18" s="55" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT18" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU18" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV18" s="57" t="n">
+        <v>1</v>
+      </c>
+      <c r="AW18" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX18" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY18" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ18" s="65" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA18" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB18" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC18" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD18" s="57" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE18" s="61" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="113"/>
-      <c r="B19" s="86" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="45" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="45" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="45" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="H19" s="66" t="n">
-        <v>0</v>
-      </c>
-      <c r="I19" s="106" t="n">
-        <v>1</v>
-      </c>
-      <c r="J19" s="66" t="n">
-        <v>0</v>
-      </c>
-      <c r="K19" s="66" t="n">
-        <v>0</v>
-      </c>
-      <c r="L19" s="66" t="n">
-        <v>1</v>
-      </c>
-      <c r="M19" s="106" t="s">
-        <v>75</v>
-      </c>
-      <c r="N19" s="106"/>
-      <c r="O19" s="106"/>
-      <c r="P19" s="70" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q19" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="R19" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="S19" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="T19" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="U19" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="V19" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="W19" s="114" t="n">
-        <v>0</v>
-      </c>
-      <c r="X19" s="70" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y19" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z19" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA19" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB19" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC19" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD19" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE19" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF19" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG19" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH19" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI19" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ19" s="47" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK19" s="46" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL19" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM19" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN19" s="47" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO19" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP19" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ19" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR19" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AS19" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT19" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU19" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV19" s="47" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW19" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX19" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY19" s="68" t="s">
-        <v>37</v>
-      </c>
-      <c r="AZ19" s="120" t="s">
-        <v>37</v>
-      </c>
-      <c r="BA19" s="46" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB19" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="BC19" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD19" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="BE19" s="47" t="n">
+      <c r="A19" s="78"/>
+      <c r="B19" s="118" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" s="119" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="118" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="118" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="118" t="s">
+        <v>37</v>
+      </c>
+      <c r="G19" s="120" t="s">
+        <v>37</v>
+      </c>
+      <c r="H19" s="52" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" s="119" t="n">
+        <v>1</v>
+      </c>
+      <c r="J19" s="118" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" s="118" t="n">
+        <v>1</v>
+      </c>
+      <c r="L19" s="120" t="n">
+        <v>1</v>
+      </c>
+      <c r="M19" s="121" t="s">
+        <v>43</v>
+      </c>
+      <c r="N19" s="121"/>
+      <c r="O19" s="121"/>
+      <c r="P19" s="119" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q19" s="119"/>
+      <c r="R19" s="119"/>
+      <c r="S19" s="119"/>
+      <c r="T19" s="119"/>
+      <c r="U19" s="119"/>
+      <c r="V19" s="119"/>
+      <c r="W19" s="119"/>
+      <c r="X19" s="122" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="118" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="118" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC19" s="118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD19" s="118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE19" s="118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF19" s="118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG19" s="118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH19" s="118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI19" s="118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ19" s="120" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK19" s="119" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL19" s="118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM19" s="118" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN19" s="120" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO19" s="119" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP19" s="118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ19" s="118" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR19" s="120" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS19" s="119" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT19" s="118" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU19" s="118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV19" s="120" t="n">
+        <v>1</v>
+      </c>
+      <c r="AW19" s="121" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX19" s="118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY19" s="52" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ19" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA19" s="119" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB19" s="118" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC19" s="118" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD19" s="120" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE19" s="120" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="78" t="n">
-        <v>8</v>
-      </c>
-      <c r="B20" s="61" t="s">
-        <v>79</v>
+        <v>9</v>
+      </c>
+      <c r="B20" s="123" t="s">
+        <v>83</v>
       </c>
       <c r="C20" s="55" t="s">
         <v>37</v>
@@ -4387,25 +4374,25 @@
       <c r="D20" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="56" t="s">
-        <v>37</v>
-      </c>
-      <c r="F20" s="56" t="s">
-        <v>37</v>
-      </c>
-      <c r="G20" s="57" t="s">
-        <v>37</v>
-      </c>
-      <c r="H20" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="I20" s="55" t="n">
-        <v>1</v>
-      </c>
-      <c r="J20" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="K20" s="56" t="n">
+      <c r="E20" s="97" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="97" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20" s="98" t="s">
+        <v>37</v>
+      </c>
+      <c r="H20" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" s="97" t="n">
+        <v>1</v>
+      </c>
+      <c r="J20" s="97" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" s="97" t="n">
         <v>1</v>
       </c>
       <c r="L20" s="57" t="n">
@@ -4416,17 +4403,31 @@
       </c>
       <c r="N20" s="61"/>
       <c r="O20" s="61"/>
-      <c r="P20" s="55" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q20" s="55"/>
-      <c r="R20" s="55"/>
-      <c r="S20" s="55"/>
-      <c r="T20" s="55"/>
-      <c r="U20" s="55"/>
-      <c r="V20" s="55"/>
-      <c r="W20" s="55"/>
-      <c r="X20" s="121" t="n">
+      <c r="P20" s="97" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q20" s="97" t="s">
+        <v>37</v>
+      </c>
+      <c r="R20" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="S20" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="T20" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="U20" s="97" t="s">
+        <v>37</v>
+      </c>
+      <c r="V20" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="W20" s="57" t="s">
+        <v>37</v>
+      </c>
+      <c r="X20" s="124" t="n">
         <v>0</v>
       </c>
       <c r="Y20" s="56" t="n">
@@ -4436,24 +4437,24 @@
         <v>0</v>
       </c>
       <c r="AA20" s="56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB20" s="56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC20" s="56" t="n">
         <v>0</v>
       </c>
-      <c r="AD20" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE20" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF20" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG20" s="56" t="n">
+      <c r="AD20" s="97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE20" s="97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF20" s="97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG20" s="97" t="n">
         <v>0</v>
       </c>
       <c r="AH20" s="56" t="n">
@@ -4472,7 +4473,7 @@
         <v>1</v>
       </c>
       <c r="AM20" s="56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN20" s="57" t="n">
         <v>1</v>
@@ -4481,7 +4482,7 @@
         <v>1</v>
       </c>
       <c r="AP20" s="56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ20" s="56" t="n">
         <v>0</v>
@@ -4490,36 +4491,36 @@
         <v>1</v>
       </c>
       <c r="AS20" s="55" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT20" s="56" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU20" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV20" s="57" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AT20" s="56" t="s">
+        <v>57</v>
+      </c>
+      <c r="AU20" s="56" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV20" s="57" t="s">
+        <v>59</v>
       </c>
       <c r="AW20" s="61" t="n">
         <v>1</v>
       </c>
-      <c r="AX20" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY20" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="AZ20" s="65" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA20" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB20" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC20" s="56" t="n">
+      <c r="AX20" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY20" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ20" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA20" s="125" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB20" s="97" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC20" s="97" t="n">
         <v>0</v>
       </c>
       <c r="BD20" s="57" t="n">
@@ -4531,133 +4532,147 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="78"/>
-      <c r="B21" s="122" t="s">
-        <v>81</v>
-      </c>
-      <c r="C21" s="123" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" s="122" t="s">
-        <v>37</v>
-      </c>
-      <c r="E21" s="122" t="s">
-        <v>37</v>
-      </c>
-      <c r="F21" s="122" t="s">
-        <v>37</v>
-      </c>
-      <c r="G21" s="124" t="s">
+      <c r="B21" s="126" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" s="119" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="118" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" s="118" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" s="118" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21" s="120" t="s">
         <v>37</v>
       </c>
       <c r="H21" s="52" t="n">
         <v>0</v>
       </c>
-      <c r="I21" s="123" t="n">
-        <v>1</v>
-      </c>
-      <c r="J21" s="122" t="n">
-        <v>0</v>
-      </c>
-      <c r="K21" s="122" t="n">
-        <v>1</v>
-      </c>
-      <c r="L21" s="124" t="n">
-        <v>1</v>
-      </c>
-      <c r="M21" s="125" t="s">
+      <c r="I21" s="119" t="n">
+        <v>1</v>
+      </c>
+      <c r="J21" s="118" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" s="118" t="n">
+        <v>1</v>
+      </c>
+      <c r="L21" s="118" t="n">
+        <v>1</v>
+      </c>
+      <c r="M21" s="121" t="s">
         <v>43</v>
       </c>
-      <c r="N21" s="125"/>
-      <c r="O21" s="125"/>
-      <c r="P21" s="123" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q21" s="123"/>
-      <c r="R21" s="123"/>
-      <c r="S21" s="123"/>
-      <c r="T21" s="123"/>
-      <c r="U21" s="123"/>
-      <c r="V21" s="123"/>
-      <c r="W21" s="123"/>
-      <c r="X21" s="126" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y21" s="122" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z21" s="122" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA21" s="122" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB21" s="122" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC21" s="122" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD21" s="122" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE21" s="122" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF21" s="122" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG21" s="122" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH21" s="122" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI21" s="122" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ21" s="124" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK21" s="123" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL21" s="122" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM21" s="122" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN21" s="124" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO21" s="123" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP21" s="122" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ21" s="122" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR21" s="124" t="n">
-        <v>1</v>
-      </c>
-      <c r="AS21" s="123" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT21" s="122" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU21" s="122" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV21" s="124" t="n">
-        <v>1</v>
-      </c>
-      <c r="AW21" s="125" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX21" s="122" t="n">
+      <c r="N21" s="121"/>
+      <c r="O21" s="121"/>
+      <c r="P21" s="119" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q21" s="118" t="s">
+        <v>37</v>
+      </c>
+      <c r="R21" s="118" t="s">
+        <v>37</v>
+      </c>
+      <c r="S21" s="118" t="s">
+        <v>37</v>
+      </c>
+      <c r="T21" s="118" t="s">
+        <v>37</v>
+      </c>
+      <c r="U21" s="118" t="s">
+        <v>37</v>
+      </c>
+      <c r="V21" s="118" t="s">
+        <v>37</v>
+      </c>
+      <c r="W21" s="118" t="s">
+        <v>37</v>
+      </c>
+      <c r="X21" s="127" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="118" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="118" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB21" s="118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC21" s="118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD21" s="118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE21" s="118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF21" s="118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG21" s="118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH21" s="118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI21" s="118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ21" s="120" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK21" s="128" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL21" s="118" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM21" s="118" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN21" s="120" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO21" s="119" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP21" s="118" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ21" s="118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR21" s="120" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS21" s="119" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT21" s="129" t="s">
+        <v>57</v>
+      </c>
+      <c r="AU21" s="129" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV21" s="130" t="s">
+        <v>59</v>
+      </c>
+      <c r="AW21" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX21" s="118" t="n">
         <v>0</v>
       </c>
       <c r="AY21" s="52" t="n">
@@ -4666,657 +4681,663 @@
       <c r="AZ21" s="53" t="n">
         <v>0</v>
       </c>
-      <c r="BA21" s="123" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB21" s="122" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC21" s="122" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD21" s="124" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE21" s="124" t="n">
+      <c r="BA21" s="119" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB21" s="118" t="n">
+        <v>1</v>
+      </c>
+      <c r="BC21" s="118" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD21" s="120" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE21" s="120" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="78" t="n">
-        <v>9</v>
-      </c>
-      <c r="B22" s="127" t="s">
-        <v>82</v>
-      </c>
-      <c r="C22" s="55" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="56" t="s">
-        <v>37</v>
-      </c>
-      <c r="E22" s="97" t="s">
-        <v>37</v>
-      </c>
-      <c r="F22" s="97" t="s">
-        <v>37</v>
-      </c>
-      <c r="G22" s="98" t="s">
-        <v>37</v>
-      </c>
-      <c r="H22" s="62" t="n">
-        <v>0</v>
-      </c>
-      <c r="I22" s="97" t="n">
-        <v>1</v>
-      </c>
-      <c r="J22" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="K22" s="97" t="n">
-        <v>1</v>
-      </c>
-      <c r="L22" s="57" t="n">
-        <v>0</v>
-      </c>
-      <c r="M22" s="61" t="s">
-        <v>43</v>
-      </c>
-      <c r="N22" s="61"/>
-      <c r="O22" s="61"/>
-      <c r="P22" s="97" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q22" s="97" t="s">
-        <v>37</v>
-      </c>
-      <c r="R22" s="56" t="s">
-        <v>37</v>
-      </c>
-      <c r="S22" s="56" t="s">
-        <v>37</v>
-      </c>
-      <c r="T22" s="56" t="s">
-        <v>37</v>
-      </c>
-      <c r="U22" s="97" t="s">
-        <v>37</v>
-      </c>
-      <c r="V22" s="56" t="s">
-        <v>37</v>
-      </c>
-      <c r="W22" s="57" t="s">
-        <v>37</v>
-      </c>
-      <c r="X22" s="128" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y22" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z22" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA22" s="56" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB22" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC22" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD22" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE22" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF22" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG22" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH22" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI22" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ22" s="57" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK22" s="55" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL22" s="56" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM22" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN22" s="57" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO22" s="55" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP22" s="56" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ22" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR22" s="57" t="n">
-        <v>1</v>
-      </c>
-      <c r="AS22" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT22" s="56" t="s">
-        <v>57</v>
-      </c>
-      <c r="AU22" s="56" t="s">
-        <v>58</v>
-      </c>
-      <c r="AV22" s="57" t="s">
-        <v>59</v>
-      </c>
-      <c r="AW22" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX22" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY22" s="62" t="n">
-        <v>0</v>
-      </c>
-      <c r="AZ22" s="60" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA22" s="118" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB22" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC22" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD22" s="57" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE22" s="61" t="n">
+      <c r="A22" s="131" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="101" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="132" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="101" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" s="101" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" s="101" t="s">
+        <v>37</v>
+      </c>
+      <c r="G22" s="133" t="s">
+        <v>37</v>
+      </c>
+      <c r="H22" s="134" t="n">
+        <v>1</v>
+      </c>
+      <c r="I22" s="135" t="s">
+        <v>86</v>
+      </c>
+      <c r="J22" s="135"/>
+      <c r="K22" s="135"/>
+      <c r="L22" s="135"/>
+      <c r="M22" s="135"/>
+      <c r="N22" s="135"/>
+      <c r="O22" s="135"/>
+      <c r="P22" s="135"/>
+      <c r="Q22" s="135"/>
+      <c r="R22" s="135"/>
+      <c r="S22" s="135"/>
+      <c r="T22" s="135"/>
+      <c r="U22" s="135"/>
+      <c r="V22" s="135"/>
+      <c r="W22" s="135"/>
+      <c r="X22" s="136" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="101" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA22" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD22" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE22" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF22" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG22" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH22" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI22" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ22" s="133" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK22" s="137" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL22" s="138" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM22" s="138" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN22" s="139" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO22" s="137" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP22" s="138" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ22" s="138" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR22" s="139" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS22" s="137" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT22" s="138" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU22" s="138" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV22" s="139" t="n">
+        <v>1</v>
+      </c>
+      <c r="AW22" s="134" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX22" s="138" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY22" s="134" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ22" s="107" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA22" s="137" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB22" s="138" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC22" s="138" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD22" s="139" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE22" s="139" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="78"/>
-      <c r="B23" s="129" t="s">
-        <v>83</v>
-      </c>
-      <c r="C23" s="123" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="E23" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="F23" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="G23" s="124" t="s">
-        <v>37</v>
-      </c>
-      <c r="H23" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="I23" s="123" t="n">
-        <v>1</v>
-      </c>
-      <c r="J23" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="K23" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="L23" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="M23" s="125" t="s">
-        <v>43</v>
-      </c>
-      <c r="N23" s="125"/>
-      <c r="O23" s="125"/>
-      <c r="P23" s="123" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q23" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="R23" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="S23" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="T23" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="U23" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="V23" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="W23" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="X23" s="130" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y23" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z23" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA23" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB23" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC23" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD23" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE23" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF23" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG23" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH23" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI23" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ23" s="124" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK23" s="131" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL23" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM23" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN23" s="124" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO23" s="123" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP23" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ23" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR23" s="124" t="n">
-        <v>1</v>
-      </c>
-      <c r="AS23" s="123" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT23" s="132" t="s">
-        <v>57</v>
-      </c>
-      <c r="AU23" s="132" t="s">
-        <v>58</v>
-      </c>
-      <c r="AV23" s="133" t="s">
-        <v>59</v>
-      </c>
-      <c r="AW23" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX23" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY23" s="52" t="n">
-        <v>0</v>
+      <c r="A23" s="111" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="140" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" s="141" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="140" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="140" t="s">
+        <v>37</v>
+      </c>
+      <c r="F23" s="140" t="s">
+        <v>37</v>
+      </c>
+      <c r="G23" s="142" t="s">
+        <v>37</v>
+      </c>
+      <c r="H23" s="143" t="n">
+        <v>1</v>
+      </c>
+      <c r="I23" s="141" t="s">
+        <v>86</v>
+      </c>
+      <c r="J23" s="141"/>
+      <c r="K23" s="141"/>
+      <c r="L23" s="141"/>
+      <c r="M23" s="141"/>
+      <c r="N23" s="141"/>
+      <c r="O23" s="141"/>
+      <c r="P23" s="141"/>
+      <c r="Q23" s="141"/>
+      <c r="R23" s="141"/>
+      <c r="S23" s="141"/>
+      <c r="T23" s="141"/>
+      <c r="U23" s="141"/>
+      <c r="V23" s="141"/>
+      <c r="W23" s="141"/>
+      <c r="X23" s="122" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="140" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z23" s="140" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="140" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="140" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="140" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD23" s="140" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE23" s="140" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF23" s="140" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG23" s="140" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH23" s="140" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI23" s="140" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ23" s="142" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK23" s="141" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL23" s="140" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM23" s="140" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN23" s="142" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO23" s="141" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP23" s="140" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ23" s="140" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR23" s="142" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS23" s="141" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT23" s="140" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU23" s="140" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV23" s="142" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW23" s="143" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX23" s="140" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY23" s="143" t="n">
+        <v>1</v>
       </c>
       <c r="AZ23" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA23" s="123" t="n">
-        <v>1</v>
-      </c>
-      <c r="BB23" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="BC23" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD23" s="124" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE23" s="124" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA23" s="141" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB23" s="140" t="n">
+        <v>1</v>
+      </c>
+      <c r="BC23" s="140" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD23" s="142" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE23" s="142" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="134" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="101" t="s">
-        <v>84</v>
-      </c>
-      <c r="C24" s="135" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" s="101" t="s">
-        <v>37</v>
-      </c>
-      <c r="E24" s="101" t="s">
-        <v>37</v>
-      </c>
-      <c r="F24" s="101" t="s">
-        <v>37</v>
-      </c>
-      <c r="G24" s="136" t="s">
-        <v>37</v>
-      </c>
-      <c r="H24" s="137" t="n">
-        <v>1</v>
-      </c>
-      <c r="I24" s="138" t="s">
-        <v>85</v>
-      </c>
-      <c r="J24" s="138"/>
-      <c r="K24" s="138"/>
-      <c r="L24" s="138"/>
-      <c r="M24" s="138"/>
-      <c r="N24" s="138"/>
-      <c r="O24" s="138"/>
-      <c r="P24" s="138"/>
-      <c r="Q24" s="138"/>
-      <c r="R24" s="138"/>
-      <c r="S24" s="138"/>
-      <c r="T24" s="138"/>
-      <c r="U24" s="138"/>
-      <c r="V24" s="138"/>
-      <c r="W24" s="138"/>
-      <c r="X24" s="139" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y24" s="101" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z24" s="101" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA24" s="101" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB24" s="101" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC24" s="101" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD24" s="101" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE24" s="101" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF24" s="101" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG24" s="101" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH24" s="101" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI24" s="101" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ24" s="136" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK24" s="140" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL24" s="141" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM24" s="141" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN24" s="142" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO24" s="140" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP24" s="141" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ24" s="141" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR24" s="142" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS24" s="140" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT24" s="141" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU24" s="141" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV24" s="142" t="n">
-        <v>1</v>
-      </c>
-      <c r="AW24" s="137" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX24" s="141" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY24" s="137" t="n">
-        <v>0</v>
-      </c>
-      <c r="AZ24" s="107" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA24" s="140" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB24" s="141" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC24" s="141" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD24" s="142" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE24" s="142" t="n">
+      <c r="A24" s="111" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="144" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" s="145" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" s="97" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" s="97" t="s">
+        <v>37</v>
+      </c>
+      <c r="F24" s="97" t="s">
+        <v>37</v>
+      </c>
+      <c r="G24" s="146" t="s">
+        <v>37</v>
+      </c>
+      <c r="H24" s="97" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" s="147" t="s">
+        <v>37</v>
+      </c>
+      <c r="J24" s="97" t="s">
+        <v>37</v>
+      </c>
+      <c r="K24" s="97" t="s">
+        <v>37</v>
+      </c>
+      <c r="L24" s="97" t="s">
+        <v>37</v>
+      </c>
+      <c r="M24" s="97" t="s">
+        <v>37</v>
+      </c>
+      <c r="N24" s="97" t="s">
+        <v>37</v>
+      </c>
+      <c r="O24" s="97" t="s">
+        <v>37</v>
+      </c>
+      <c r="P24" s="97" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q24" s="97" t="s">
+        <v>37</v>
+      </c>
+      <c r="R24" s="97" t="s">
+        <v>37</v>
+      </c>
+      <c r="S24" s="97" t="s">
+        <v>37</v>
+      </c>
+      <c r="T24" s="97" t="s">
+        <v>37</v>
+      </c>
+      <c r="U24" s="97" t="s">
+        <v>37</v>
+      </c>
+      <c r="V24" s="97" t="s">
+        <v>37</v>
+      </c>
+      <c r="W24" s="146" t="s">
+        <v>37</v>
+      </c>
+      <c r="X24" s="147" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y24" s="97" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA24" s="97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB24" s="97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC24" s="97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD24" s="97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE24" s="97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF24" s="97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG24" s="97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH24" s="97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI24" s="97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ24" s="146" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK24" s="148" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL24" s="97" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM24" s="97" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN24" s="146" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO24" s="148" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP24" s="97" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ24" s="97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR24" s="146" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS24" s="148" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT24" s="97" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU24" s="97" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV24" s="146" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW24" s="149" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX24" s="149" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY24" s="97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ24" s="150" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA24" s="63" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB24" s="97" t="n">
+        <v>1</v>
+      </c>
+      <c r="BC24" s="97" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD24" s="146" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE24" s="146" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="111" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" s="143" t="s">
-        <v>86</v>
-      </c>
-      <c r="C25" s="144" t="s">
-        <v>37</v>
-      </c>
-      <c r="D25" s="143" t="s">
-        <v>37</v>
-      </c>
-      <c r="E25" s="143" t="s">
-        <v>37</v>
-      </c>
-      <c r="F25" s="143" t="s">
-        <v>37</v>
-      </c>
-      <c r="G25" s="145" t="s">
-        <v>37</v>
-      </c>
-      <c r="H25" s="146" t="n">
-        <v>1</v>
-      </c>
-      <c r="I25" s="144" t="s">
-        <v>85</v>
-      </c>
-      <c r="J25" s="144"/>
-      <c r="K25" s="144"/>
-      <c r="L25" s="144"/>
-      <c r="M25" s="144"/>
-      <c r="N25" s="144"/>
-      <c r="O25" s="144"/>
-      <c r="P25" s="144"/>
-      <c r="Q25" s="144"/>
-      <c r="R25" s="144"/>
-      <c r="S25" s="144"/>
-      <c r="T25" s="144"/>
-      <c r="U25" s="144"/>
-      <c r="V25" s="144"/>
-      <c r="W25" s="144"/>
-      <c r="X25" s="126" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y25" s="143" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z25" s="143" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA25" s="143" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB25" s="143" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC25" s="143" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD25" s="143" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE25" s="143" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF25" s="143" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG25" s="143" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH25" s="143" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI25" s="143" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ25" s="145" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK25" s="144" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL25" s="143" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM25" s="143" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN25" s="145" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO25" s="144" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP25" s="143" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ25" s="143" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR25" s="145" t="n">
-        <v>1</v>
-      </c>
-      <c r="AS25" s="144" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT25" s="143" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU25" s="143" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV25" s="145" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW25" s="146" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX25" s="143" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY25" s="146" t="n">
-        <v>1</v>
-      </c>
-      <c r="AZ25" s="53" t="n">
-        <v>1</v>
-      </c>
-      <c r="BA25" s="144" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB25" s="143" t="n">
-        <v>1</v>
-      </c>
-      <c r="BC25" s="143" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD25" s="145" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE25" s="145" t="n">
+      <c r="A25" s="111"/>
+      <c r="B25" s="151" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" s="96" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="G25" s="114" t="s">
+        <v>37</v>
+      </c>
+      <c r="H25" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" s="70" t="s">
+        <v>37</v>
+      </c>
+      <c r="J25" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="K25" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="L25" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="M25" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="N25" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="O25" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="P25" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q25" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="R25" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="S25" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="T25" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="U25" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="V25" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="W25" s="114" t="s">
+        <v>37</v>
+      </c>
+      <c r="X25" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y25" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA25" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB25" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC25" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD25" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE25" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF25" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG25" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH25" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI25" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ25" s="114" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK25" s="96" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL25" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM25" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN25" s="114" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO25" s="96" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP25" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ25" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR25" s="114" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS25" s="96" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT25" s="45" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU25" s="45" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV25" s="114" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW25" s="152" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX25" s="152" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY25" s="45" t="n">
+        <v>1</v>
+      </c>
+      <c r="AZ25" s="106" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA25" s="153" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB25" s="45" t="n">
+        <v>1</v>
+      </c>
+      <c r="BC25" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD25" s="114" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE25" s="114" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="111" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26" s="147" t="s">
-        <v>87</v>
-      </c>
-      <c r="C26" s="148" t="n">
-        <v>0</v>
+      <c r="A26" s="111"/>
+      <c r="B26" s="144" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" s="147" t="n">
+        <v>1</v>
       </c>
       <c r="D26" s="97" t="s">
         <v>37</v>
@@ -5327,13 +5348,13 @@
       <c r="F26" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="G26" s="117" t="s">
-        <v>37</v>
-      </c>
-      <c r="H26" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="I26" s="116" t="s">
+      <c r="G26" s="146" t="s">
+        <v>37</v>
+      </c>
+      <c r="H26" s="154" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" s="147" t="s">
         <v>37</v>
       </c>
       <c r="J26" s="97" t="s">
@@ -5346,14 +5367,10 @@
         <v>37</v>
       </c>
       <c r="M26" s="97" t="s">
-        <v>37</v>
-      </c>
-      <c r="N26" s="97" t="s">
-        <v>37</v>
-      </c>
-      <c r="O26" s="97" t="s">
-        <v>37</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="N26" s="97"/>
+      <c r="O26" s="97"/>
       <c r="P26" s="97" t="s">
         <v>37</v>
       </c>
@@ -5375,10 +5392,10 @@
       <c r="V26" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="W26" s="117" t="s">
-        <v>37</v>
-      </c>
-      <c r="X26" s="116" t="n">
+      <c r="W26" s="146" t="s">
+        <v>37</v>
+      </c>
+      <c r="X26" s="147" t="n">
         <v>1</v>
       </c>
       <c r="Y26" s="97" t="n">
@@ -5414,10 +5431,10 @@
       <c r="AI26" s="97" t="n">
         <v>0</v>
       </c>
-      <c r="AJ26" s="117" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK26" s="149" t="n">
+      <c r="AJ26" s="146" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK26" s="147" t="n">
         <v>1</v>
       </c>
       <c r="AL26" s="97" t="n">
@@ -5426,22 +5443,22 @@
       <c r="AM26" s="97" t="n">
         <v>1</v>
       </c>
-      <c r="AN26" s="117" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO26" s="149" t="n">
+      <c r="AN26" s="146" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO26" s="147" t="n">
         <v>1</v>
       </c>
       <c r="AP26" s="97" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ26" s="97" t="n">
         <v>0</v>
       </c>
-      <c r="AR26" s="117" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS26" s="149" t="n">
+      <c r="AR26" s="146" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS26" s="147" t="n">
         <v>1</v>
       </c>
       <c r="AT26" s="97" t="n">
@@ -5450,22 +5467,22 @@
       <c r="AU26" s="97" t="n">
         <v>1</v>
       </c>
-      <c r="AV26" s="117" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW26" s="150" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX26" s="150" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY26" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AZ26" s="115" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA26" s="63" t="n">
+      <c r="AV26" s="146" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW26" s="154" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX26" s="154" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY26" s="149" t="n">
+        <v>1</v>
+      </c>
+      <c r="AZ26" s="144" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA26" s="147" t="n">
         <v>0</v>
       </c>
       <c r="BB26" s="97" t="n">
@@ -5474,524 +5491,186 @@
       <c r="BC26" s="97" t="n">
         <v>0</v>
       </c>
-      <c r="BD26" s="117" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE26" s="117" t="n">
+      <c r="BD26" s="146" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE26" s="146" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="111"/>
-      <c r="B27" s="151" t="s">
-        <v>88</v>
-      </c>
-      <c r="C27" s="96" t="n">
-        <v>1</v>
-      </c>
-      <c r="D27" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="E27" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="F27" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="G27" s="114" t="s">
-        <v>37</v>
-      </c>
-      <c r="H27" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="I27" s="70" t="s">
-        <v>37</v>
-      </c>
-      <c r="J27" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="K27" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="L27" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="M27" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="N27" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="O27" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="P27" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q27" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="R27" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="S27" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="T27" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="U27" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="V27" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="W27" s="114" t="s">
-        <v>37</v>
-      </c>
-      <c r="X27" s="70" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y27" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z27" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA27" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB27" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC27" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD27" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE27" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF27" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG27" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH27" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI27" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ27" s="114" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK27" s="96" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL27" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM27" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN27" s="114" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO27" s="96" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP27" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ27" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR27" s="114" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS27" s="96" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT27" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU27" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV27" s="114" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW27" s="152" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX27" s="152" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY27" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="AZ27" s="106" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA27" s="153" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB27" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="BC27" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD27" s="114" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE27" s="114" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="111"/>
-      <c r="B28" s="147" t="s">
-        <v>89</v>
-      </c>
-      <c r="C28" s="116" t="n">
-        <v>1</v>
-      </c>
-      <c r="D28" s="97" t="s">
-        <v>37</v>
-      </c>
-      <c r="E28" s="97" t="s">
-        <v>37</v>
-      </c>
-      <c r="F28" s="97" t="s">
-        <v>37</v>
-      </c>
-      <c r="G28" s="117" t="s">
-        <v>37</v>
-      </c>
-      <c r="H28" s="154" t="n">
-        <v>0</v>
-      </c>
-      <c r="I28" s="116" t="s">
-        <v>37</v>
-      </c>
-      <c r="J28" s="97" t="s">
-        <v>37</v>
-      </c>
-      <c r="K28" s="97" t="s">
-        <v>37</v>
-      </c>
-      <c r="L28" s="97" t="s">
-        <v>37</v>
-      </c>
-      <c r="M28" s="97" t="s">
-        <v>75</v>
-      </c>
-      <c r="N28" s="97"/>
-      <c r="O28" s="97"/>
-      <c r="P28" s="97" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q28" s="97" t="s">
-        <v>37</v>
-      </c>
-      <c r="R28" s="97" t="s">
-        <v>37</v>
-      </c>
-      <c r="S28" s="97" t="s">
-        <v>37</v>
-      </c>
-      <c r="T28" s="97" t="s">
-        <v>37</v>
-      </c>
-      <c r="U28" s="97" t="s">
-        <v>37</v>
-      </c>
-      <c r="V28" s="97" t="s">
-        <v>37</v>
-      </c>
-      <c r="W28" s="117" t="s">
-        <v>37</v>
-      </c>
-      <c r="X28" s="116" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y28" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z28" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA28" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB28" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC28" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD28" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE28" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF28" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG28" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH28" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI28" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ28" s="117" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK28" s="116" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL28" s="97" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM28" s="97" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN28" s="117" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO28" s="116" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP28" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ28" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR28" s="117" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS28" s="116" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT28" s="97" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU28" s="97" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV28" s="117" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW28" s="154" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX28" s="154" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY28" s="150" t="n">
-        <v>1</v>
-      </c>
-      <c r="AZ28" s="147" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA28" s="116" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB28" s="97" t="n">
-        <v>1</v>
-      </c>
-      <c r="BC28" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD28" s="117" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE28" s="117" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="111"/>
-      <c r="B29" s="155" t="s">
-        <v>90</v>
-      </c>
-      <c r="C29" s="156" t="n">
-        <v>1</v>
-      </c>
-      <c r="D29" s="157" t="s">
-        <v>37</v>
-      </c>
-      <c r="E29" s="157" t="s">
-        <v>37</v>
-      </c>
-      <c r="F29" s="157" t="s">
-        <v>37</v>
-      </c>
-      <c r="G29" s="158" t="s">
-        <v>37</v>
-      </c>
-      <c r="H29" s="159" t="n">
-        <v>1</v>
-      </c>
-      <c r="I29" s="156" t="n">
-        <v>0</v>
-      </c>
-      <c r="J29" s="157" t="n">
-        <v>0</v>
-      </c>
-      <c r="K29" s="157" t="n">
-        <v>0</v>
-      </c>
-      <c r="L29" s="157" t="n">
-        <v>0</v>
-      </c>
-      <c r="M29" s="157" t="n">
-        <v>0</v>
-      </c>
-      <c r="N29" s="157" t="n">
-        <v>0</v>
-      </c>
-      <c r="O29" s="157" t="n">
-        <v>0</v>
-      </c>
-      <c r="P29" s="157" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="157" t="n">
-        <v>0</v>
-      </c>
-      <c r="R29" s="157" t="n">
-        <v>0</v>
-      </c>
-      <c r="S29" s="157" t="n">
-        <v>0</v>
-      </c>
-      <c r="T29" s="157" t="n">
-        <v>0</v>
-      </c>
-      <c r="U29" s="157" t="n">
-        <v>0</v>
-      </c>
-      <c r="V29" s="157" t="n">
-        <v>0</v>
-      </c>
-      <c r="W29" s="158" t="n">
-        <v>0</v>
-      </c>
-      <c r="X29" s="156" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y29" s="157" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z29" s="157" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA29" s="157" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB29" s="157" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC29" s="157" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD29" s="157" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE29" s="157" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF29" s="157" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG29" s="157" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH29" s="157" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI29" s="157" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ29" s="158" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK29" s="156" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL29" s="157" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM29" s="157" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN29" s="158" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO29" s="156" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP29" s="157" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ29" s="157" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR29" s="158" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS29" s="156" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT29" s="157" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU29" s="157" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV29" s="158" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW29" s="159" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX29" s="159" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY29" s="160" t="n">
-        <v>1</v>
-      </c>
-      <c r="AZ29" s="155" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA29" s="156" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB29" s="157" t="n">
-        <v>1</v>
-      </c>
-      <c r="BC29" s="157" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD29" s="158" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE29" s="158" t="n">
+      <c r="B27" s="155" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" s="156" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" s="157" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" s="157" t="s">
+        <v>37</v>
+      </c>
+      <c r="F27" s="157" t="s">
+        <v>37</v>
+      </c>
+      <c r="G27" s="158" t="s">
+        <v>37</v>
+      </c>
+      <c r="H27" s="159" t="n">
+        <v>1</v>
+      </c>
+      <c r="I27" s="156" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" s="157" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" s="157" t="n">
+        <v>0</v>
+      </c>
+      <c r="L27" s="157" t="n">
+        <v>0</v>
+      </c>
+      <c r="M27" s="157" t="n">
+        <v>0</v>
+      </c>
+      <c r="N27" s="157" t="n">
+        <v>0</v>
+      </c>
+      <c r="O27" s="157" t="n">
+        <v>0</v>
+      </c>
+      <c r="P27" s="157" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="157" t="n">
+        <v>0</v>
+      </c>
+      <c r="R27" s="157" t="n">
+        <v>0</v>
+      </c>
+      <c r="S27" s="157" t="n">
+        <v>0</v>
+      </c>
+      <c r="T27" s="157" t="n">
+        <v>0</v>
+      </c>
+      <c r="U27" s="157" t="n">
+        <v>0</v>
+      </c>
+      <c r="V27" s="157" t="n">
+        <v>0</v>
+      </c>
+      <c r="W27" s="158" t="n">
+        <v>0</v>
+      </c>
+      <c r="X27" s="156" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y27" s="157" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z27" s="157" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA27" s="157" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="157" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC27" s="157" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD27" s="157" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE27" s="157" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF27" s="157" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG27" s="157" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH27" s="157" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI27" s="157" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ27" s="158" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK27" s="156" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL27" s="157" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM27" s="157" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN27" s="158" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO27" s="156" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP27" s="157" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ27" s="157" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR27" s="158" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS27" s="156" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT27" s="157" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU27" s="157" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV27" s="158" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW27" s="159" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX27" s="159" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY27" s="160" t="n">
+        <v>1</v>
+      </c>
+      <c r="AZ27" s="155" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA27" s="156" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB27" s="157" t="n">
+        <v>1</v>
+      </c>
+      <c r="BC27" s="157" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD27" s="158" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE27" s="158" t="n">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="58">
+  <mergeCells count="55">
     <mergeCell ref="A1:B3"/>
     <mergeCell ref="C1:G2"/>
     <mergeCell ref="H1:W2"/>
@@ -6035,21 +5714,18 @@
     <mergeCell ref="D16:G16"/>
     <mergeCell ref="M16:O16"/>
     <mergeCell ref="P16:W16"/>
-    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A18:A19"/>
     <mergeCell ref="M18:O18"/>
+    <mergeCell ref="P18:W18"/>
     <mergeCell ref="M19:O19"/>
+    <mergeCell ref="P19:W19"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="M20:O20"/>
-    <mergeCell ref="P20:W20"/>
     <mergeCell ref="M21:O21"/>
-    <mergeCell ref="P21:W21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="M22:O22"/>
-    <mergeCell ref="M23:O23"/>
-    <mergeCell ref="I24:W24"/>
-    <mergeCell ref="I25:W25"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="M28:O28"/>
+    <mergeCell ref="I22:W22"/>
+    <mergeCell ref="I23:W23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="M26:O26"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>